<commit_message>
Some visual details added
</commit_message>
<xml_diff>
--- a/Bid data.xlsx
+++ b/Bid data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Storage\Github\TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D29171F-2D62-4F74-AAA5-0896E52D0C60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D344F-6F3A-46FD-B291-FECF1FA9FED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{C5DF7C8C-8BD2-41CE-8E3D-7A07E42A8EF2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="13">
   <si>
     <t>Firm</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Firm10</t>
-  </si>
-  <si>
-    <t>Fir3</t>
   </si>
 </sst>
 </file>
@@ -116,37 +113,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -469,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7405B2E-B17D-4055-8E5D-E9D2B359F3AF}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58:K58"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1668,7 @@
         <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1">
         <v>93</v>
@@ -3603,7 +3570,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Firm7"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
The probability is correctly calculated now
</commit_message>
<xml_diff>
--- a/Bid data.xlsx
+++ b/Bid data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Storage\Github\TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D344F-6F3A-46FD-B291-FECF1FA9FED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD6E985-523D-450C-9628-B372193D8AE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{C5DF7C8C-8BD2-41CE-8E3D-7A07E42A8EF2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="13">
   <si>
     <t>Firm</t>
   </si>
@@ -436,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7405B2E-B17D-4055-8E5D-E9D2B359F3AF}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="N80" sqref="A76:N80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,31 +2577,37 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C69" s="1">
-        <v>98</v>
+        <v>210000</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E69" s="1">
-        <v>86</v>
+        <v>215000</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
-        <v>89</v>
+        <v>220000</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I69" s="1">
-        <v>114</v>
+        <v>230000</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K69" s="1">
+        <v>200000</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>